<commit_message>
docs: update spreadsheet files
</commit_message>
<xml_diff>
--- a/HyperIndex-Revenue Expense Calculator.xlsx
+++ b/HyperIndex-Revenue Expense Calculator.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/48d8db5c7a2c79dd/문서/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="827" documentId="6_{5A323E48-DD3B-4DD7-85A9-3D8430E72DB1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E250C8D2-9F07-438B-9B9F-2AA532C34518}"/>
+  <xr:revisionPtr revIDLastSave="850" documentId="6_{5A323E48-DD3B-4DD7-85A9-3D8430E72DB1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{06794A90-4182-4526-87CA-7843EDAE2A17}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="13900" activeTab="2" xr2:uid="{FC9F7C52-8CC4-43B2-A95D-05CC98FBD406}"/>
   </bookViews>
@@ -930,7 +930,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="98">
+  <cellXfs count="99">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1223,6 +1223,9 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="180" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -2011,16 +2014,16 @@
             <c:numRef>
               <c:f>'Net Income Calculator'!$B$3:$B$5</c:f>
               <c:numCache>
-                <c:formatCode>_(* #,##0_);_(* \(#,##0\);_(* "-"_);_(@_)</c:formatCode>
+                <c:formatCode>_-* #,##0.00_-;\-* #,##0.00_-;_-* "-"_-;_-@_-</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>137.37613642245762</c:v>
+                  <c:v>5.1516051158421607</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>49.724229773168425</c:v>
+                  <c:v>5.3967796037042106</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>87.651906649289202</c:v>
+                  <c:v>-0.24517448786204987</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2175,7 +2178,7 @@
             </a:p>
           </c:txPr>
         </c:title>
-        <c:numFmt formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)" sourceLinked="1"/>
+        <c:numFmt formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;_-;_-@_-" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -2486,22 +2489,22 @@
             <c:numRef>
               <c:f>'Net Income Calculator'!$B$6:$B$10</c:f>
               <c:numCache>
-                <c:formatCode>0%</c:formatCode>
+                <c:formatCode>_-* #,##0.00_-;\-* #,##0.00_-;_-* "-"_-;_-@_-</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>0.63804317789039433</c:v>
+                  <c:v>-4.7591863574343446E-2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>9.3120015016642618E-2</c:v>
+                  <c:v>0.68666099001628189</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.92123600516895432</c:v>
+                  <c:v>0.31829920452626698</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2.7085386865594918E-2</c:v>
+                  <c:v>9.3583588192733807E-3</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.33344765684390304</c:v>
+                  <c:v>0.3334476568439031</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2598,7 +2601,7 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
-        <c:numFmt formatCode="0%" sourceLinked="1"/>
+        <c:numFmt formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;_-;_-@_-" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -2903,10 +2906,10 @@
                 <c:formatCode>_(* #,##0_);_(* \(#,##0\);_(* "-"_);_(@_)</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)">
-                  <c:v>40860.085264036017</c:v>
+                  <c:v>20000</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>45000</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3211,10 +3214,10 @@
                 <c:formatCode>_(* #,##0_);_(* \(#,##0\);_(* "-"_);_(@_)</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>4423455.4177284967</c:v>
+                  <c:v>20000</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>657389.29986966902</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -6292,7 +6295,7 @@
       </c>
       <c r="G2">
         <f>'Net Income Calculator'!B2</f>
-        <v>20</v>
+        <v>0.75</v>
       </c>
       <c r="J2" t="s">
         <v>101</v>
@@ -6397,7 +6400,7 @@
       <c r="F5" s="8"/>
       <c r="G5">
         <f>G2*0.25</f>
-        <v>5</v>
+        <v>0.1875</v>
       </c>
       <c r="H5" s="2"/>
       <c r="J5" s="2" t="s">
@@ -6437,23 +6440,23 @@
       </c>
       <c r="K6" s="47">
         <f>B12*K4/(K3*K2)</f>
-        <v>1.020833333333333</v>
+        <v>3.8281249999999989E-2</v>
       </c>
       <c r="L6" s="47">
         <f>C12*L4/(L3*L2)</f>
-        <v>0.40384615384615385</v>
+        <v>1.5144230769230766E-2</v>
       </c>
       <c r="M6" s="47">
         <f>M4*E12/(M3*M2)</f>
-        <v>4.8582995951417011E-2</v>
+        <v>1.8218623481781376E-3</v>
       </c>
       <c r="N6" s="47">
         <f>N4*(F14+F14*N4)/(N3*N2)</f>
-        <v>1.6027397260273971E-2</v>
+        <v>6.010273972602739E-4</v>
       </c>
       <c r="O6">
         <f>D14*O5/365</f>
-        <v>3.287671232876712E-2</v>
+        <v>1.2328767123287671E-3</v>
       </c>
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.45">
@@ -6480,11 +6483,11 @@
       </c>
       <c r="K7" s="51">
         <f>B12/K6</f>
-        <v>1.7142857142857149</v>
+        <v>1.7142857142857144</v>
       </c>
       <c r="L7" s="51">
         <f>C12/L6</f>
-        <v>4.333333333333333</v>
+        <v>4.3333333333333339</v>
       </c>
       <c r="M7" s="51">
         <f>E12/M6</f>
@@ -6496,7 +6499,7 @@
       </c>
       <c r="O7" s="51">
         <f>D14/O6</f>
-        <v>182.50000000000003</v>
+        <v>182.5</v>
       </c>
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.45">
@@ -6573,11 +6576,11 @@
       </c>
       <c r="K10">
         <f>G2*B13*3/4</f>
-        <v>3</v>
+        <v>0.11250000000000002</v>
       </c>
       <c r="L10">
         <f>B14-표9[[#This Row],[Internal Volume (B)]]</f>
-        <v>1</v>
+        <v>3.7500000000000006E-2</v>
       </c>
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.45">
@@ -6604,11 +6607,11 @@
       </c>
       <c r="K11">
         <f>G2*C13*(17/25)</f>
-        <v>3.4000000000000004</v>
+        <v>0.1275</v>
       </c>
       <c r="L11">
         <f>C14-표9[[#This Row],[Internal Volume (B)]]</f>
-        <v>1.5999999999999996</v>
+        <v>0.06</v>
       </c>
     </row>
     <row r="12" spans="1:19" x14ac:dyDescent="0.45">
@@ -6617,18 +6620,18 @@
       </c>
       <c r="B12" s="21">
         <f>B11*G5</f>
-        <v>1.75</v>
+        <v>6.5624999999999989E-2</v>
       </c>
       <c r="C12" s="21">
         <f>G5*C11</f>
-        <v>1.75</v>
+        <v>6.5624999999999989E-2</v>
       </c>
       <c r="D12" s="21">
         <v>0</v>
       </c>
       <c r="E12" s="21">
         <f>E11*G5</f>
-        <v>1.5</v>
+        <v>5.6249999999999994E-2</v>
       </c>
       <c r="F12" s="21">
         <v>0</v>
@@ -6638,11 +6641,11 @@
       </c>
       <c r="K12">
         <f>G2*D13*(14/30)</f>
-        <v>2.8</v>
+        <v>0.105</v>
       </c>
       <c r="L12">
         <f>D14-표9[[#This Row],[Internal Volume (B)]]</f>
-        <v>3.2</v>
+        <v>0.11999999999999998</v>
       </c>
       <c r="M12" s="48"/>
       <c r="N12" s="48"/>
@@ -6672,11 +6675,11 @@
       </c>
       <c r="K13">
         <f>G2*표4[[#This Row],[VS Theme]]*(8/10)</f>
-        <v>1.6</v>
+        <v>6.0000000000000012E-2</v>
       </c>
       <c r="L13">
         <f>E14-표9[[#This Row],[Internal Volume (B)]]</f>
-        <v>0.39999999999999991</v>
+        <v>1.4999999999999999E-2</v>
       </c>
       <c r="M13" s="46"/>
       <c r="N13" s="46"/>
@@ -6689,23 +6692,23 @@
       </c>
       <c r="B14" s="13">
         <f>G2*B13</f>
-        <v>4</v>
+        <v>0.15000000000000002</v>
       </c>
       <c r="C14" s="13">
         <f>G2*C13</f>
-        <v>5</v>
+        <v>0.1875</v>
       </c>
       <c r="D14" s="13">
         <f>G2*D13</f>
-        <v>6</v>
+        <v>0.22499999999999998</v>
       </c>
       <c r="E14" s="13">
         <f>G2*E13</f>
-        <v>2</v>
+        <v>7.5000000000000011E-2</v>
       </c>
       <c r="F14" s="13">
         <f>G2*F13</f>
-        <v>3</v>
+        <v>0.11249999999999999</v>
       </c>
       <c r="I14" s="3"/>
       <c r="J14" t="s">
@@ -6713,11 +6716,11 @@
       </c>
       <c r="K14">
         <f>SUM(K10:K13)</f>
-        <v>10.799999999999999</v>
+        <v>0.40500000000000003</v>
       </c>
       <c r="L14">
         <f>SUM(L10:L13)</f>
-        <v>6.1999999999999993</v>
+        <v>0.23249999999999998</v>
       </c>
       <c r="M14" s="46"/>
       <c r="N14" s="46"/>
@@ -6730,15 +6733,15 @@
       </c>
       <c r="B15" s="15">
         <f>K7</f>
-        <v>1.7142857142857149</v>
+        <v>1.7142857142857144</v>
       </c>
       <c r="C15" s="15">
         <f>L7</f>
-        <v>4.333333333333333</v>
+        <v>4.3333333333333339</v>
       </c>
       <c r="D15" s="15">
         <f>O7</f>
-        <v>182.50000000000003</v>
+        <v>182.5</v>
       </c>
       <c r="E15" s="15">
         <f>M7</f>
@@ -6759,23 +6762,23 @@
       </c>
       <c r="B16" s="21">
         <f>K6</f>
-        <v>1.020833333333333</v>
+        <v>3.8281249999999989E-2</v>
       </c>
       <c r="C16" s="21">
         <f>L6</f>
-        <v>0.40384615384615385</v>
+        <v>1.5144230769230766E-2</v>
       </c>
       <c r="D16" s="50">
         <f t="shared" ref="D16:F16" si="0">M6</f>
-        <v>4.8582995951417011E-2</v>
+        <v>1.8218623481781376E-3</v>
       </c>
       <c r="E16" s="50">
         <f t="shared" si="0"/>
-        <v>1.6027397260273971E-2</v>
+        <v>6.010273972602739E-4</v>
       </c>
       <c r="F16" s="50">
         <f t="shared" si="0"/>
-        <v>3.287671232876712E-2</v>
+        <v>1.2328767123287671E-3</v>
       </c>
       <c r="I16" s="3"/>
       <c r="J16" t="s">
@@ -6802,7 +6805,7 @@
       </c>
       <c r="K17" s="49">
         <f>F14</f>
-        <v>3</v>
+        <v>0.11249999999999999</v>
       </c>
       <c r="L17" s="46"/>
       <c r="M17" s="46"/>
@@ -6872,7 +6875,7 @@
       </c>
       <c r="K20">
         <f>SUM(K10+K13+K11)</f>
-        <v>8</v>
+        <v>0.30000000000000004</v>
       </c>
       <c r="L20" s="45"/>
       <c r="M20" s="46"/>
@@ -6904,7 +6907,7 @@
       </c>
       <c r="K21">
         <f>K12</f>
-        <v>2.8</v>
+        <v>0.105</v>
       </c>
       <c r="L21" s="45"/>
       <c r="M21" s="46"/>
@@ -6918,30 +6921,30 @@
       </c>
       <c r="B22" s="53">
         <f>K20*65%</f>
-        <v>5.2</v>
+        <v>0.19500000000000003</v>
       </c>
       <c r="C22" s="53">
         <f>K20*35%</f>
-        <v>2.8</v>
+        <v>0.10500000000000001</v>
       </c>
       <c r="D22" s="53">
         <f>K21</f>
-        <v>2.8</v>
+        <v>0.105</v>
       </c>
       <c r="E22" s="53">
         <f>K22</f>
-        <v>6.1999999999999993</v>
+        <v>0.23249999999999998</v>
       </c>
       <c r="F22" s="53">
         <f>K23</f>
-        <v>3</v>
+        <v>0.11249999999999999</v>
       </c>
       <c r="J22" t="s">
         <v>117</v>
       </c>
       <c r="K22">
         <f>SUM(L10:L13)</f>
-        <v>6.1999999999999993</v>
+        <v>0.23249999999999998</v>
       </c>
       <c r="L22" s="45"/>
       <c r="M22" s="46"/>
@@ -6955,7 +6958,7 @@
       </c>
       <c r="K23" cm="1">
         <f t="array" ref="K23">표12[Volume(B)]</f>
-        <v>3</v>
+        <v>0.11249999999999999</v>
       </c>
       <c r="L23" s="45"/>
       <c r="M23" s="46"/>
@@ -7015,11 +7018,11 @@
       </c>
       <c r="C28" s="16" cm="1">
         <f t="array" ref="C28">표6[HOOATS - Orderbook Internal]*D2*1000</f>
-        <v>23.27</v>
+        <v>0.8726250000000001</v>
       </c>
       <c r="D28" s="1">
         <f>C28/C33</f>
-        <v>0.24668716209053324</v>
+        <v>0.24668716209053326</v>
       </c>
       <c r="E28" s="1">
         <f>C28/C49</f>
@@ -7038,15 +7041,15 @@
       </c>
       <c r="C29" s="16" cm="1">
         <f t="array" ref="C29">D2*표6[HOOATS - AMM Internal]*1000</f>
-        <v>12.53</v>
+        <v>0.46987500000000004</v>
       </c>
       <c r="D29" s="1">
         <f>C29/C33</f>
-        <v>0.13283154881797943</v>
+        <v>0.13283154881797946</v>
       </c>
       <c r="E29" s="1">
         <f>C29/C49</f>
-        <v>9.1209436560858559E-2</v>
+        <v>9.1209436560858573E-2</v>
       </c>
       <c r="L29" s="45"/>
       <c r="M29" s="46"/>
@@ -7061,7 +7064,7 @@
       </c>
       <c r="C30" s="16" cm="1">
         <f t="array" ref="C30">표6[Bonding Curve Internal]*D2*1000</f>
-        <v>12.53</v>
+        <v>0.46987499999999999</v>
       </c>
       <c r="D30" s="1">
         <f>C30/C33</f>
@@ -7084,7 +7087,7 @@
       </c>
       <c r="C31" s="16" cm="1">
         <f t="array" ref="C31">표6[Partner Indices]*E2*1000</f>
-        <v>15</v>
+        <v>0.5625</v>
       </c>
       <c r="D31" s="1">
         <f>표10[[#This Row],[Amount (M)]]/C33</f>
@@ -7107,7 +7110,7 @@
       </c>
       <c r="C32" s="16" cm="1">
         <f t="array" ref="C32">F2*1000*표6[Partner Routing]</f>
-        <v>30.999999999999996</v>
+        <v>1.1624999999999999</v>
       </c>
       <c r="D32" s="1">
         <f>C32/C33</f>
@@ -7130,7 +7133,7 @@
       </c>
       <c r="C33" s="82">
         <f>SUM(C28:C32)</f>
-        <v>94.33</v>
+        <v>3.5373749999999999</v>
       </c>
       <c r="D33" s="19"/>
       <c r="E33" s="19">
@@ -7166,15 +7169,15 @@
       </c>
       <c r="C35" s="16">
         <f>B16*B8*12*1000</f>
-        <v>12.249999999999996</v>
+        <v>0.45937499999999992</v>
       </c>
       <c r="D35" s="1">
         <f>C35/C39</f>
-        <v>0.39443447116890212</v>
+        <v>0.39443447116890218</v>
       </c>
       <c r="E35" s="1">
         <f>C35/C49</f>
-        <v>8.9171236861174549E-2</v>
+        <v>8.9171236861174563E-2</v>
       </c>
       <c r="L35" s="45"/>
       <c r="M35" s="46"/>
@@ -7189,15 +7192,15 @@
       </c>
       <c r="C36" s="16">
         <f>C8*C16*26*1000</f>
-        <v>10.5</v>
+        <v>0.39374999999999988</v>
       </c>
       <c r="D36" s="1">
         <f>C36/C39</f>
-        <v>0.33808668957334481</v>
+        <v>0.33808668957334465</v>
       </c>
       <c r="E36" s="1">
         <f>C36/C49</f>
-        <v>7.6432488738149632E-2</v>
+        <v>7.6432488738149618E-2</v>
       </c>
       <c r="L36" s="45"/>
       <c r="M36" s="46"/>
@@ -7212,7 +7215,7 @@
       </c>
       <c r="C37" s="16">
         <f>F16*F8*12*1000</f>
-        <v>7.8904109589041092</v>
+        <v>0.29589041095890412</v>
       </c>
       <c r="D37" s="1">
         <f>C37/C39</f>
@@ -7220,7 +7223,7 @@
       </c>
       <c r="E37" s="1">
         <f>C37/C49</f>
-        <v>5.7436547310077218E-2</v>
+        <v>5.7436547310077225E-2</v>
       </c>
       <c r="L37" s="45"/>
       <c r="M37" s="46"/>
@@ -7235,15 +7238,15 @@
       </c>
       <c r="C38" s="16">
         <f>E8*26*1000*E16</f>
-        <v>0.41671232876712333</v>
+        <v>1.5626712328767122E-2</v>
       </c>
       <c r="D38" s="1">
         <f>C38/C39</f>
-        <v>1.341760873688343E-2</v>
+        <v>1.3417608736883427E-2</v>
       </c>
       <c r="E38" s="1">
         <f>C38/C49</f>
-        <v>3.0333676548134534E-3</v>
+        <v>3.0333676548134529E-3</v>
       </c>
       <c r="P38" s="46"/>
     </row>
@@ -7254,7 +7257,7 @@
       </c>
       <c r="C39" s="82">
         <f>SUM(C35:C38)</f>
-        <v>31.057123287671228</v>
+        <v>1.1646421232876711</v>
       </c>
       <c r="D39" s="19"/>
       <c r="E39" s="19">
@@ -7277,11 +7280,11 @@
       </c>
       <c r="C41" s="16">
         <f>B9*B16*1000</f>
-        <v>7.1458333333333313</v>
+        <v>0.26796874999999992</v>
       </c>
       <c r="D41" s="1">
         <f>C41/C46</f>
-        <v>0.62743217948421126</v>
+        <v>0.62743217948421137</v>
       </c>
       <c r="E41" s="1">
         <f>C41/C49</f>
@@ -7300,15 +7303,15 @@
       </c>
       <c r="C42" s="16">
         <f>C16*C9*1000</f>
-        <v>3.4326923076923079</v>
+        <v>0.1287259615384615</v>
       </c>
       <c r="D42" s="1">
         <f>C42/C46</f>
-        <v>0.30140384132208592</v>
+        <v>0.30140384132208586</v>
       </c>
       <c r="E42" s="1">
         <f>C42/C49</f>
-        <v>2.4987544395164304E-2</v>
+        <v>2.4987544395164298E-2</v>
       </c>
       <c r="I42" s="12"/>
       <c r="J42" s="14"/>
@@ -7324,7 +7327,7 @@
       </c>
       <c r="C43" s="16">
         <f>E9*E16*1000</f>
-        <v>0.16027397260273973</v>
+        <v>6.0102739726027388E-3</v>
       </c>
       <c r="D43" s="1">
         <f>C43/C46</f>
@@ -7332,7 +7335,7 @@
       </c>
       <c r="E43" s="1">
         <f>C43/C49</f>
-        <v>1.1666798672359435E-3</v>
+        <v>1.1666798672359433E-3</v>
       </c>
       <c r="I43" s="12"/>
       <c r="J43" s="21"/>
@@ -7348,11 +7351,11 @@
       </c>
       <c r="C44" s="16">
         <f>F9*F16*1000</f>
-        <v>0.16438356164383561</v>
+        <v>6.1643835616438354E-3</v>
       </c>
       <c r="D44" s="1">
         <f>C44/C46</f>
-        <v>1.4433521122365341E-2</v>
+        <v>1.4433521122365345E-2</v>
       </c>
       <c r="E44" s="1">
         <f>C44/C49</f>
@@ -7372,15 +7375,15 @@
       </c>
       <c r="C45" s="16">
         <f>D9*D16*1000</f>
-        <v>0.48582995951417013</v>
+        <v>1.8218623481781378E-2</v>
       </c>
       <c r="D45" s="1">
         <f>C45/C46</f>
-        <v>4.2657774977031181E-2</v>
+        <v>4.2657774977031188E-2</v>
       </c>
       <c r="E45" s="1">
         <f>C45/C49</f>
-        <v>3.5364945627830956E-3</v>
+        <v>3.5364945627830951E-3</v>
       </c>
       <c r="I45" s="12"/>
       <c r="J45" s="13"/>
@@ -7396,12 +7399,12 @@
       </c>
       <c r="C46" s="82">
         <f>SUM(C41:C45)</f>
-        <v>11.389013134786385</v>
+        <v>0.42708799255448937</v>
       </c>
       <c r="D46" s="19"/>
       <c r="E46" s="19">
         <f>C46/C49</f>
-        <v>8.2903868396495106E-2</v>
+        <v>8.2903868396495092E-2</v>
       </c>
       <c r="I46" s="12"/>
       <c r="J46" s="15"/>
@@ -7431,7 +7434,7 @@
       </c>
       <c r="C48" s="82">
         <f>5*'Net Income Calculator'!B11*12/1000000</f>
-        <v>0.6</v>
+        <v>2.2499999999999999E-2</v>
       </c>
       <c r="D48" s="19"/>
       <c r="E48" s="19">
@@ -7447,7 +7450,7 @@
       <c r="B49" s="58"/>
       <c r="C49" s="83">
         <f>C48+C46+C39+C33</f>
-        <v>137.37613642245762</v>
+        <v>5.1516051158421607</v>
       </c>
       <c r="D49" s="59"/>
       <c r="E49" s="59">
@@ -7944,7 +7947,7 @@
   <dimension ref="A1:W75"/>
   <sheetViews>
     <sheetView topLeftCell="A30" zoomScale="61" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="H36" sqref="H36"/>
+      <selection activeCell="C66" sqref="C66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.45"/>
@@ -8330,7 +8333,7 @@
       </c>
       <c r="C32" s="16">
         <f>(Revenue!C28+Revenue!C29+Revenue!C30+Revenue!C31*50%)*F4</f>
-        <v>25.744608750000001</v>
+        <v>0.96542282812500013</v>
       </c>
       <c r="D32" s="44">
         <f>C32/C37</f>
@@ -8338,7 +8341,7 @@
       </c>
       <c r="E32" s="2">
         <f>C32/C65</f>
-        <v>0.51774776336288253</v>
+        <v>0.1788886889993356</v>
       </c>
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.45">
@@ -8348,7 +8351,7 @@
       </c>
       <c r="C33" s="16">
         <f>Revenue!C32*Expense!B22</f>
-        <v>16.352499999999996</v>
+        <v>0.61321874999999992</v>
       </c>
       <c r="D33" s="44">
         <f>C33/C37</f>
@@ -8356,7 +8359,7 @@
       </c>
       <c r="E33" s="2">
         <f>표10_19[[#This Row],[Amount (M)]]/C65</f>
-        <v>0.32886381698815031</v>
+        <v>0.11362679135147605</v>
       </c>
       <c r="G33" s="81"/>
       <c r="H33" s="55"/>
@@ -8369,7 +8372,7 @@
       </c>
       <c r="C34" s="16">
         <f>SUM(D26*C26+D27*C27)*'Net Income Calculator'!B12*55%/100</f>
-        <v>1.65</v>
+        <v>6.1875000000000006E-2</v>
       </c>
       <c r="D34" s="2">
         <f>C34/C37</f>
@@ -8377,7 +8380,7 @@
       </c>
       <c r="E34" s="2">
         <f>표10_19[[#This Row],[Amount (M)]]/C65</f>
-        <v>3.3183017766729744E-2</v>
+        <v>1.1465170813633116E-2</v>
       </c>
       <c r="G34" s="57"/>
       <c r="H34" s="56"/>
@@ -8390,15 +8393,15 @@
       </c>
       <c r="C35" s="41">
         <f>2*'Net Income Calculator'!B2/100</f>
-        <v>0.4</v>
+        <v>1.4999999999999999E-2</v>
       </c>
       <c r="D35" s="2">
         <f>C35/C37</f>
-        <v>8.9994605104657139E-3</v>
+        <v>8.9994605104657122E-3</v>
       </c>
       <c r="E35" s="2">
         <f>표10_19[[#This Row],[Amount (M)]]/C65</f>
-        <v>8.0443679434496363E-3</v>
+        <v>2.7794353487595428E-3</v>
       </c>
       <c r="G35" s="57" t="s">
         <v>146</v>
@@ -8415,23 +8418,23 @@
       </c>
       <c r="C36" s="16">
         <f>1.5*'Net Income Calculator'!B2/100</f>
-        <v>0.3</v>
+        <v>1.125E-2</v>
       </c>
       <c r="D36" s="2">
         <f>C36/C37</f>
-        <v>6.749595382849285E-3</v>
+        <v>6.7495953828492841E-3</v>
       </c>
       <c r="E36" s="2">
         <f>표10_19[[#This Row],[Amount (M)]]/C65</f>
-        <v>6.0332759575872259E-3</v>
+        <v>2.0845765115696572E-3</v>
       </c>
       <c r="G36" s="92">
         <f>Revenue!C49*0.01%*15*1000000</f>
-        <v>206064.20463368643</v>
+        <v>7727.4076737632422</v>
       </c>
       <c r="H36" s="93">
         <f>Revenue!C49*0.1%*1000000+J38</f>
-        <v>163440.34105614407</v>
+        <v>12879.012789605404</v>
       </c>
       <c r="I36" s="56"/>
     </row>
@@ -8442,12 +8445,12 @@
       </c>
       <c r="C37" s="61">
         <f>SUM(C32:C36)</f>
-        <v>44.447108749999991</v>
+        <v>1.6667665781249998</v>
       </c>
       <c r="D37" s="62"/>
       <c r="E37" s="62">
         <f>표10_19[[#This Row],[Amount (M)]]/C65</f>
-        <v>0.89387224201879933</v>
+        <v>0.30884466302477392</v>
       </c>
       <c r="G37" s="57" t="s">
         <v>148</v>
@@ -8471,19 +8474,19 @@
       <c r="E38" s="2"/>
       <c r="G38" s="94">
         <f>IF(H36&lt;80000, 80000, H36)</f>
-        <v>163440.34105614407</v>
+        <v>80000</v>
       </c>
       <c r="H38">
         <f>INT(G36 / 45000)</f>
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="I38" s="85">
         <f xml:space="preserve"> INT(G36/ 45000) * 45000</f>
-        <v>180000</v>
+        <v>0</v>
       </c>
       <c r="J38" s="47">
         <f xml:space="preserve"> G36 - (INT(G36 / 45000) * 45000)</f>
-        <v>26064.20463368643</v>
+        <v>7727.4076737632422</v>
       </c>
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.45">
@@ -8497,11 +8500,11 @@
       </c>
       <c r="D39" s="2">
         <f>C39/C41</f>
-        <v>0.89285714285714279</v>
+        <v>0.99552015928322546</v>
       </c>
       <c r="E39" s="2">
         <f>표10_19[[#This Row],[Amount (M)]]/C65</f>
-        <v>3.6199655745523356E-2</v>
+        <v>0.33353224185114511</v>
       </c>
       <c r="G39" t="s">
         <v>152</v>
@@ -8517,23 +8520,23 @@
       </c>
       <c r="C40" s="16">
         <f>(0.2*4+0.0125*3.5*4+0.0035*7.5*4)*'Net Income Calculator'!B2/100</f>
-        <v>0.21600000000000003</v>
+        <v>8.1000000000000013E-3</v>
       </c>
       <c r="D40" s="2">
         <f>C40/C41</f>
-        <v>0.10714285714285715</v>
+        <v>4.4798407167745162E-3</v>
       </c>
       <c r="E40" s="2">
         <f>표10_19[[#This Row],[Amount (M)]]/C65</f>
-        <v>4.3439586894628039E-3</v>
+        <v>1.5008950883301534E-3</v>
       </c>
       <c r="G40" s="47">
         <f>G38/4</f>
-        <v>40860.085264036017</v>
-      </c>
-      <c r="I40" s="85">
+        <v>20000</v>
+      </c>
+      <c r="I40" s="85" t="e">
         <f>I38/H38</f>
-        <v>45000</v>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="41" spans="1:10" s="11" customFormat="1" x14ac:dyDescent="0.45">
@@ -8543,12 +8546,12 @@
       </c>
       <c r="C41" s="61">
         <f>SUM(C39:C40)</f>
-        <v>2.016</v>
+        <v>1.8080999999999998</v>
       </c>
       <c r="D41" s="62"/>
       <c r="E41" s="62">
         <f>표10_19[[#This Row],[Amount (M)]]/C65</f>
-        <v>4.0543614434986164E-2</v>
+        <v>0.33503313693947528</v>
       </c>
       <c r="G41"/>
     </row>
@@ -8571,11 +8574,11 @@
       </c>
       <c r="D43" s="2">
         <f>C43/C56</f>
-        <v>0.6963788300835656</v>
+        <v>18.570102135561751</v>
       </c>
       <c r="E43" s="2">
         <f>표10_19[[#This Row],[Amount (M)]]/C65</f>
-        <v>6.0332759575872277E-3</v>
+        <v>5.5588706975190867E-2</v>
       </c>
     </row>
     <row r="44" spans="1:10" x14ac:dyDescent="0.45">
@@ -8589,11 +8592,11 @@
       </c>
       <c r="D44" s="2">
         <f>C44/C56</f>
-        <v>0.4178272980501393</v>
+        <v>11.142061281337048</v>
       </c>
       <c r="E44" s="2">
         <f>표10_19[[#This Row],[Amount (M)]]/C65</f>
-        <v>3.6199655745523356E-3</v>
+        <v>3.3353224185114515E-2</v>
       </c>
     </row>
     <row r="45" spans="1:10" x14ac:dyDescent="0.45">
@@ -8607,11 +8610,11 @@
       </c>
       <c r="D45" s="2">
         <f>C45/C56</f>
-        <v>0.11142061281337048</v>
+        <v>2.9712163416898796</v>
       </c>
       <c r="E45" s="2">
         <f>표10_19[[#This Row],[Amount (M)]]/C65</f>
-        <v>9.6532415321395621E-4</v>
+        <v>8.8941931160305375E-3</v>
       </c>
     </row>
     <row r="46" spans="1:10" x14ac:dyDescent="0.45">
@@ -8629,7 +8632,7 @@
       </c>
       <c r="E46" s="2">
         <f>표10_19[[#This Row],[Amount (M)]]/C65</f>
-        <v>3.6199655745523362E-4</v>
+        <v>3.335322418511452E-3</v>
       </c>
     </row>
     <row r="47" spans="1:10" x14ac:dyDescent="0.45">
@@ -8643,11 +8646,11 @@
       </c>
       <c r="D47" s="77">
         <f>C47/C56</f>
-        <v>1.5320334261838442</v>
+        <v>40.854224698235846</v>
       </c>
       <c r="E47" s="78">
         <f>표10_19[[#This Row],[Amount (M)]]/C65</f>
-        <v>1.3273207106691899E-2</v>
+        <v>0.12229515534541989</v>
       </c>
     </row>
     <row r="48" spans="1:10" x14ac:dyDescent="0.45">
@@ -8661,11 +8664,11 @@
       </c>
       <c r="D48" s="80">
         <f>C48/C56</f>
-        <v>0.6963788300835656</v>
+        <v>18.570102135561751</v>
       </c>
       <c r="E48" s="80">
         <f>표10_19[[#This Row],[Amount (M)]]/C65</f>
-        <v>6.0332759575872277E-3</v>
+        <v>5.5588706975190867E-2</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.45">
@@ -8679,11 +8682,11 @@
       </c>
       <c r="D49" s="2">
         <f>C49/C56</f>
-        <v>1.0027855153203342</v>
+        <v>26.740947075208911</v>
       </c>
       <c r="E49" s="2">
         <f>표10_19[[#This Row],[Amount (M)]]/C65</f>
-        <v>8.6879173789256043E-3</v>
+        <v>8.0047738044274827E-2</v>
       </c>
       <c r="F49" s="9"/>
     </row>
@@ -8698,11 +8701,11 @@
       </c>
       <c r="D50" s="2">
         <f>C50/C56</f>
-        <v>0.1392757660167131</v>
+        <v>3.7140204271123491</v>
       </c>
       <c r="E50" s="2">
         <f>표10_19[[#This Row],[Amount (M)]]/C65</f>
-        <v>1.2066551915174452E-3</v>
+        <v>1.1117741395038171E-2</v>
       </c>
       <c r="F50" s="33"/>
     </row>
@@ -8717,11 +8720,11 @@
       </c>
       <c r="D51" s="2">
         <f>C51/C56</f>
-        <v>0.1392757660167131</v>
+        <v>3.7140204271123491</v>
       </c>
       <c r="E51" s="2">
         <f>표10_19[[#This Row],[Amount (M)]]/C65</f>
-        <v>1.2066551915174452E-3</v>
+        <v>1.1117741395038171E-2</v>
       </c>
       <c r="F51" s="12"/>
     </row>
@@ -8736,11 +8739,11 @@
       </c>
       <c r="D52" s="2">
         <f>C52/C56</f>
-        <v>8.356545961002787E-2</v>
+        <v>2.22841225626741</v>
       </c>
       <c r="E52" s="2">
         <f>표10_19[[#This Row],[Amount (M)]]/C65</f>
-        <v>7.2399311491046724E-4</v>
+        <v>6.670644837022904E-3</v>
       </c>
       <c r="F52" s="13"/>
     </row>
@@ -8755,11 +8758,11 @@
       </c>
       <c r="D53" s="2">
         <f>C53/C56</f>
-        <v>0.1392757660167131</v>
+        <v>3.7140204271123491</v>
       </c>
       <c r="E53" s="2">
         <f>표10_19[[#This Row],[Amount (M)]]/C65</f>
-        <v>1.2066551915174452E-3</v>
+        <v>1.1117741395038171E-2</v>
       </c>
       <c r="F53" s="34"/>
     </row>
@@ -8774,11 +8777,11 @@
       </c>
       <c r="D54" s="2">
         <f>C54/C56</f>
-        <v>0.55710306406685239</v>
+        <v>14.856081708449397</v>
       </c>
       <c r="E54" s="2">
         <f>표10_19[[#This Row],[Amount (M)]]/C65</f>
-        <v>4.8266207660697807E-3</v>
+        <v>4.4470965580152684E-2</v>
       </c>
       <c r="F54" s="15"/>
     </row>
@@ -8793,11 +8796,11 @@
       </c>
       <c r="D55" s="2">
         <f>C55/C56</f>
-        <v>0.55710306406685239</v>
+        <v>14.856081708449397</v>
       </c>
       <c r="E55" s="2">
         <f>표10_19[[#This Row],[Amount (M)]]/C65</f>
-        <v>4.8266207660697807E-3</v>
+        <v>4.4470965580152684E-2</v>
       </c>
       <c r="F55" s="35"/>
     </row>
@@ -8808,12 +8811,12 @@
       </c>
       <c r="C56" s="64">
         <f>SUM(C43:C53)*'Net Income Calculator'!B2/100</f>
-        <v>0.43079999999999996</v>
+        <v>1.6154999999999999E-2</v>
       </c>
       <c r="D56" s="65"/>
       <c r="E56" s="65">
         <f>표10_19[[#This Row],[Amount (M)]]/C65</f>
-        <v>8.6637842750952564E-3</v>
+        <v>2.9934518706140273E-3</v>
       </c>
       <c r="F56" s="39"/>
     </row>
@@ -8833,15 +8836,15 @@
       </c>
       <c r="C58" s="89">
         <f>0.5%*Revenue!C49</f>
-        <v>0.68688068211228814</v>
+        <v>2.5758025579210805E-2</v>
       </c>
       <c r="D58" s="90">
         <f>표10_19[[#This Row],[Amount (M)]]/C64</f>
-        <v>0.24268649262384817</v>
+        <v>1.3515895110231664E-2</v>
       </c>
       <c r="E58" s="91">
         <f>표10_19[[#This Row],[Amount (M)]]/C65</f>
-        <v>1.3813802350397275E-2</v>
+        <v>4.7728511206074006E-3</v>
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.45">
@@ -8860,15 +8863,15 @@
       </c>
       <c r="C60" s="36">
         <f>(G40*4+I38)/1000000</f>
-        <v>0.34344034105614407</v>
+        <v>0.08</v>
       </c>
       <c r="D60" s="33">
         <f>표10_19[[#This Row],[Amount (M)]]/C64</f>
-        <v>0.12134324631192409</v>
+        <v>4.197804701658589E-2</v>
       </c>
       <c r="E60" s="33">
         <f>표10_19[[#This Row],[Amount (M)]]/C65</f>
-        <v>6.9069011751986377E-3</v>
+        <v>1.4823655193384229E-2</v>
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.45">
@@ -8891,11 +8894,11 @@
       </c>
       <c r="D62" s="33">
         <f>표10_19[[#This Row],[Amount (M)]]/C64</f>
-        <v>0.35331681170234874</v>
+        <v>0.52472558770732358</v>
       </c>
       <c r="E62" s="33">
         <f>표10_19[[#This Row],[Amount (M)]]/C65</f>
-        <v>2.0110919858624086E-2</v>
+        <v>0.18529568991730286</v>
       </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.45">
@@ -8909,11 +8912,11 @@
       </c>
       <c r="D63" s="34">
         <f>표10_19[[#This Row],[Amount (M)]]/C64</f>
-        <v>0.28265344936187903</v>
+        <v>0.4197804701658589</v>
       </c>
       <c r="E63" s="34">
         <f>표10_19[[#This Row],[Amount (M)]]/C65</f>
-        <v>1.6088735886899273E-2</v>
+        <v>0.1482365519338423</v>
       </c>
     </row>
     <row r="64" spans="1:6" s="11" customFormat="1" x14ac:dyDescent="0.45">
@@ -8923,12 +8926,12 @@
       </c>
       <c r="C64" s="70">
         <f>SUM(C58:C63)</f>
-        <v>2.8303210231684321</v>
+        <v>1.9057580255792108</v>
       </c>
       <c r="D64" s="71"/>
       <c r="E64" s="71">
         <f>표10_19[[#This Row],[Amount (M)]]/C65</f>
-        <v>5.692035927111927E-2</v>
+        <v>0.35312874816513679</v>
       </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.45">
@@ -8938,7 +8941,7 @@
       <c r="B65" s="72"/>
       <c r="C65" s="84">
         <f>SUM(C64+C56+C41+C37)</f>
-        <v>49.724229773168425</v>
+        <v>5.3967796037042106</v>
       </c>
       <c r="D65" s="73"/>
       <c r="E65" s="74">
@@ -8952,7 +8955,7 @@
       </c>
       <c r="B67" s="47">
         <f>Revenue!C49-Expense!C65</f>
-        <v>87.651906649289202</v>
+        <v>-0.24517448786204987</v>
       </c>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.45">
@@ -9527,7 +9530,7 @@
   <dimension ref="A1:C23"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="R17" sqref="R17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.45"/>
@@ -9549,79 +9552,79 @@
         <v>136</v>
       </c>
       <c r="B2">
-        <v>20</v>
+        <v>0.75</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A3" s="94" t="s">
         <v>137</v>
       </c>
-      <c r="B3" s="94">
+      <c r="B3" s="16">
         <f>Revenue!C49</f>
-        <v>137.37613642245762</v>
+        <v>5.1516051158421607</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A4" s="94" t="s">
         <v>140</v>
       </c>
-      <c r="B4" s="94">
+      <c r="B4" s="16">
         <f>Expense!C65</f>
-        <v>49.724229773168425</v>
+        <v>5.3967796037042106</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A5" s="94" t="s">
         <v>130</v>
       </c>
-      <c r="B5" s="94">
+      <c r="B5" s="16">
         <f>Expense!B67</f>
-        <v>87.651906649289202</v>
+        <v>-0.24517448786204987</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
         <v>141</v>
       </c>
-      <c r="B6" s="86">
+      <c r="B6" s="98">
         <f>Expense!B67/Revenue!C49</f>
-        <v>0.63804317789039433</v>
+        <v>-4.7591863574343446E-2</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A7" s="86" t="s">
         <v>143</v>
       </c>
-      <c r="B7" s="86">
+      <c r="B7" s="98">
         <f>SUM(Expense!C64,Expense!C39)/B4</f>
-        <v>9.3120015016642618E-2</v>
+        <v>0.68666099001628189</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A8" s="86" t="s">
         <v>144</v>
       </c>
-      <c r="B8" s="86" cm="1">
+      <c r="B8" s="98" cm="1">
         <f t="array" ref="B8">SUM(Expense!C32:C34+Expense!C58)/B4</f>
-        <v>0.92123600516895432</v>
+        <v>0.31829920452626698</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A9" s="86" t="s">
         <v>142</v>
       </c>
-      <c r="B9" s="86">
+      <c r="B9" s="98">
         <f>SUM(Expense!C35:C36,Expense!C56,Expense!C40)/B4</f>
-        <v>2.7085386865594918E-2</v>
+        <v>9.3583588192733807E-3</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A10" s="86" t="s">
         <v>145</v>
       </c>
-      <c r="B10" s="86" cm="1">
+      <c r="B10" s="98" cm="1">
         <f t="array" ref="B10">SUM(Expense!C32:C34+Expense!C58)/B3</f>
-        <v>0.33344765684390304</v>
+        <v>0.3334476568439031</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.45">
@@ -9630,7 +9633,7 @@
       </c>
       <c r="B11" s="94">
         <f>50000*(B2/100)</f>
-        <v>10000</v>
+        <v>375</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.45">
@@ -9639,7 +9642,7 @@
       </c>
       <c r="B12" s="94">
         <f>400*(B2/100)</f>
-        <v>80</v>
+        <v>3</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.45">
@@ -9648,16 +9651,16 @@
       </c>
       <c r="B13" s="96">
         <f>Expense!G40</f>
-        <v>40860.085264036017</v>
+        <v>20000</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A14" s="86" t="s">
         <v>154</v>
       </c>
-      <c r="B14" s="97">
+      <c r="B14" s="97" t="e">
         <f>Expense!I40</f>
-        <v>45000</v>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.45">
@@ -9665,17 +9668,17 @@
         <v>157</v>
       </c>
       <c r="B15" s="94">
-        <f>B13+B5*1000000*20%/4</f>
-        <v>4423455.4177284967</v>
+        <f>IF(B13+B5*1000000*20%/4 &lt; B13, B13, B13+B5*1000000*20%/4)</f>
+        <v>20000</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A16" s="86" t="s">
         <v>158</v>
       </c>
-      <c r="B16" s="94">
-        <f>B5*1000000*3%/Expense!H38</f>
-        <v>657389.29986966902</v>
+      <c r="B16" s="94" t="e">
+        <f>IF(B5*1000000*3%/Expense!H38 &lt; B14, B14, B5*1000000*3%/Expense!H38)</f>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.45">

</xml_diff>